<commit_message>
continued to assess plate differences for ELISA, started adjusting manuscript based on comments
</commit_message>
<xml_diff>
--- a/Manuscripts/GDF15 during Pregnancy/Data and R Scripts/450 read.xlsx
+++ b/Manuscripts/GDF15 during Pregnancy/Data and R Scripts/450 read.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mollyec/Documents/GitHub/Developmental-Obesity/Manuscripts/GDF15 during Pregnancy/Data and R Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2A9540D-0E9A-1D4D-B024-03578CFA953E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D65E70-4F8E-134D-92F6-5C6271AF9642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="1000" windowWidth="24260" windowHeight="12500" xr2:uid="{A32D3030-8C5B-4B9B-A5DC-1323307EB03F}"/>
   </bookViews>
@@ -594,15 +594,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76694A8-0823-4EC1-94A1-DE510551C38B}">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6:Z13"/>
+      <selection activeCell="O6" sqref="O6:AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -732,7 +732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -849,8 +849,50 @@
       <c r="X5" s="16">
         <v>10</v>
       </c>
+      <c r="Y5" s="16">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="16">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="16">
+        <v>13</v>
+      </c>
+      <c r="AB5" s="16">
+        <v>14</v>
+      </c>
+      <c r="AC5" s="16">
+        <v>15</v>
+      </c>
+      <c r="AD5" s="16">
+        <v>16</v>
+      </c>
+      <c r="AE5" s="16">
+        <v>17</v>
+      </c>
+      <c r="AF5" s="16">
+        <v>18</v>
+      </c>
+      <c r="AG5" s="16">
+        <v>19</v>
+      </c>
+      <c r="AH5" s="16">
+        <v>20</v>
+      </c>
+      <c r="AI5" s="16">
+        <v>21</v>
+      </c>
+      <c r="AJ5" s="16">
+        <v>22</v>
+      </c>
+      <c r="AK5" s="16">
+        <v>23</v>
+      </c>
+      <c r="AL5" s="16">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -939,8 +981,44 @@
       <c r="Z6" s="5">
         <v>0</v>
       </c>
+      <c r="AA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1029,8 +1107,44 @@
       <c r="Z7" s="5">
         <v>0</v>
       </c>
+      <c r="AA7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1119,8 +1233,44 @@
       <c r="Z8" s="5">
         <v>0</v>
       </c>
+      <c r="AA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1209,8 +1359,44 @@
       <c r="Z9" s="5">
         <v>0</v>
       </c>
+      <c r="AA9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>450</v>
       </c>
@@ -1260,8 +1446,44 @@
       <c r="Z10" s="5">
         <v>0</v>
       </c>
+      <c r="AA10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -1345,8 +1567,44 @@
       <c r="Z11" s="5">
         <v>0</v>
       </c>
+      <c r="AA11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1435,8 +1693,44 @@
       <c r="Z12" s="5">
         <v>0</v>
       </c>
+      <c r="AA12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1525,8 +1819,44 @@
       <c r="Z13" s="5">
         <v>0</v>
       </c>
+      <c r="AA13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1570,7 +1900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1614,7 +1944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>